<commit_message>
Finally have User index route able to show a response. Next step is to test the other routes and then seed data to db.
</commit_message>
<xml_diff>
--- a/planning/Route-Resource-Table.xlsx
+++ b/planning/Route-Resource-Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/roger/GeneralAssembly/projects/project-2/planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8751910B-D899-8444-A96A-510CA592D5CC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988A4F83-9FB7-074D-A55E-E74760E142A9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="17540" xr2:uid="{9CFC03DA-A025-3D4F-A3EC-99D48DF078CC}"/>
   </bookViews>
@@ -883,8 +883,8 @@
   <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -969,7 +969,7 @@
       <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -986,7 +986,7 @@
       <c r="D6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1003,7 +1003,7 @@
       <c r="D7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1020,7 +1020,7 @@
       <c r="D8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1037,7 +1037,7 @@
       <c r="D9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="1" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1054,7 +1054,7 @@
       <c r="D10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1071,7 +1071,7 @@
       <c r="D11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="1" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>